<commit_message>
fix courts upload logic
</commit_message>
<xml_diff>
--- a/backend/data/courts.xlsx
+++ b/backend/data/courts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\projects\VolleyBolley\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFE5FF5-395F-42EC-B5C3-C76CD3532424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C2B344-3B6C-48BB-A2FF-00ED70712518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="116">
   <si>
     <t>country</t>
   </si>
@@ -364,6 +364,15 @@
   </si>
   <si>
     <t>Beach court in Polis</t>
+  </si>
+  <si>
+    <t>7.8804</t>
+  </si>
+  <si>
+    <t>12.9236</t>
+  </si>
+  <si>
+    <t>12.5707</t>
   </si>
 </sst>
 </file>
@@ -441,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -449,8 +458,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,7 +747,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H21"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,8 +834,8 @@
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="3">
-        <v>2521818</v>
+      <c r="B4" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>31</v>
@@ -848,8 +860,8 @@
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="3">
-        <v>2679756</v>
+      <c r="B5" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -900,8 +912,8 @@
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="3">
-        <v>1390814</v>
+      <c r="B7" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>38</v>

</xml_diff>